<commit_message>
Added the option to skip rows at the beginning. Added testcase for that.
</commit_message>
<xml_diff>
--- a/test/string_test.xlsx
+++ b/test/string_test.xlsx
@@ -20,7 +20,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t xml:space="preserve">Dies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beiden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zeilen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sollten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geskippt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">werden</t>
+  </si>
   <si>
     <t xml:space="preserve">Meine</t>
   </si>
@@ -148,15 +166,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -167,7 +185,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -187,6 +205,28 @@
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>